<commit_message>
Edited 2nd time by tester1
</commit_message>
<xml_diff>
--- a/TestData/Test_Data.xlsx
+++ b/TestData/Test_Data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="CredKart_login_Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CredKart_login_Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -410,10 +410,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="D7:E7"/>
+      <selection activeCell="A6" sqref="A6:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -560,60 +560,6 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Credencetest@test.com</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>Credence@123</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>login_pass</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>login_pass</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Credencetest@test.com1</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>Credence@1231</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>login_pass</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>login_fail</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>
@@ -623,9 +569,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B4" r:id="rId5"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A5" r:id="rId6"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A6" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A7" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B7" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>